<commit_message>
add some files in purchase attempt files
</commit_message>
<xml_diff>
--- a/admin_panel/purchase_management/purchase_attempt_logs/filter_custom_date.xlsx
+++ b/admin_panel/purchase_management/purchase_attempt_logs/filter_custom_date.xlsx
@@ -8,19 +8,19 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\SymlexVPNTestCases\admin_panel\purchase_management\purchase_attempt_logs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A82E0045-C0E6-4397-AD7B-37C6435F6DF6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79F8A339-3B86-4B03-B120-B8336EEF1EA0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="purchase _attempt_logs" sheetId="1" r:id="rId1"/>
+    <sheet name="filter_custom_date" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="57">
   <si>
     <t>Test Case ID</t>
   </si>
@@ -130,9 +130,6 @@
     <t>SYM-AP_PAL_FCD_025</t>
   </si>
   <si>
-    <t xml:space="preserve">try to expand the "filter custom date" </t>
-  </si>
-  <si>
     <t>1. go to Symlex admin panel
 2. login with proper credentials
 3. go to purchase management 
@@ -142,6 +139,63 @@
   </si>
   <si>
     <t>the expanded options will be shown</t>
+  </si>
+  <si>
+    <t>try to expand the "filter custom date" field</t>
+  </si>
+  <si>
+    <t>the payment logs should be filtered based on the selected custom date range.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">choose the "filter custom date " from this field </t>
+  </si>
+  <si>
+    <t xml:space="preserve">choose the "today " from this field </t>
+  </si>
+  <si>
+    <t xml:space="preserve">choose the "yesterday " from this field </t>
+  </si>
+  <si>
+    <t xml:space="preserve">choose the "this week " from this field </t>
+  </si>
+  <si>
+    <t xml:space="preserve">choose the "this month " from this field </t>
+  </si>
+  <si>
+    <t xml:space="preserve">choose the "last 15 days " from this field </t>
+  </si>
+  <si>
+    <t>only payment logs created in the last 15 days should be displayed.</t>
+  </si>
+  <si>
+    <t>only payment logs created within the current month should be displayed.</t>
+  </si>
+  <si>
+    <t>only payment logs created within the current week should be displayed.</t>
+  </si>
+  <si>
+    <t>only payment logs created yesterday should be displayed.</t>
+  </si>
+  <si>
+    <t>only payment logs created today should be displayed.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">choose the "last 30 days " from this field </t>
+  </si>
+  <si>
+    <t>Only records created in the last 30 days should be displayed.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">choose the "last week " from this field </t>
+  </si>
+  <si>
+    <t>Data from the previous week is displayed.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">choose the "last 7 days " from this field </t>
+  </si>
+  <si>
+    <t>only payment logs created from the last 7 days should be displayed.</t>
   </si>
 </sst>
 </file>
@@ -1019,7 +1073,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table_1" displayName="Table_1" ref="A3:G1048575" dataDxfId="7">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table_1" displayName="Table_1" ref="A3:G1048576" dataDxfId="7">
   <tableColumns count="7">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Test Case ID" dataDxfId="6"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Prerequisites" dataDxfId="5"/>
@@ -1237,15 +1291,15 @@
   <dimension ref="A1:Z990"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="79" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E5" sqref="E5"/>
+      <pane ySplit="3" topLeftCell="A29" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C33" sqref="C33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="21.109375" style="15" customWidth="1"/>
     <col min="2" max="2" width="21.109375" style="18" customWidth="1"/>
-    <col min="3" max="3" width="44.44140625" style="20" customWidth="1"/>
+    <col min="3" max="3" width="48.109375" style="20" customWidth="1"/>
     <col min="4" max="4" width="57.33203125" style="18" customWidth="1"/>
     <col min="5" max="5" width="45.6640625" style="20" customWidth="1"/>
     <col min="6" max="6" width="10.6640625" style="21" customWidth="1"/>
@@ -1359,13 +1413,13 @@
       </c>
       <c r="B4" s="10"/>
       <c r="C4" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="D4" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="D4" s="10" t="s">
+      <c r="E4" s="10" t="s">
         <v>37</v>
-      </c>
-      <c r="E4" s="10" t="s">
-        <v>38</v>
       </c>
       <c r="F4" s="6" t="s">
         <v>6</v>
@@ -1393,16 +1447,20 @@
       <c r="Y4" s="3"/>
       <c r="Z4" s="3"/>
     </row>
-    <row r="5" spans="1:26" ht="123" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:26" ht="100.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="10" t="s">
         <v>12</v>
       </c>
       <c r="B5" s="10"/>
-      <c r="C5" s="10"/>
-      <c r="D5" s="10">
-        <v>2</v>
+      <c r="C5" s="10" t="s">
+        <v>40</v>
       </c>
-      <c r="E5" s="10"/>
+      <c r="D5" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="E5" s="10" t="s">
+        <v>39</v>
+      </c>
       <c r="F5" s="6"/>
       <c r="G5" s="6"/>
       <c r="H5" s="3"/>
@@ -1430,11 +1488,15 @@
         <v>13</v>
       </c>
       <c r="B6" s="10"/>
-      <c r="C6" s="10"/>
+      <c r="C6" s="10" t="s">
+        <v>41</v>
+      </c>
       <c r="D6" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="E6" s="10"/>
+      <c r="E6" s="10" t="s">
+        <v>50</v>
+      </c>
       <c r="F6" s="6"/>
       <c r="G6" s="6"/>
       <c r="H6" s="3"/>
@@ -1462,11 +1524,15 @@
         <v>14</v>
       </c>
       <c r="B7" s="10"/>
-      <c r="C7" s="10"/>
+      <c r="C7" s="10" t="s">
+        <v>42</v>
+      </c>
       <c r="D7" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="E7" s="10"/>
+      <c r="E7" s="10" t="s">
+        <v>49</v>
+      </c>
       <c r="F7" s="6"/>
       <c r="G7" s="6"/>
       <c r="H7" s="3"/>
@@ -1494,11 +1560,15 @@
         <v>15</v>
       </c>
       <c r="B8" s="10"/>
-      <c r="C8" s="10"/>
+      <c r="C8" s="10" t="s">
+        <v>43</v>
+      </c>
       <c r="D8" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="E8" s="10"/>
+      <c r="E8" s="10" t="s">
+        <v>48</v>
+      </c>
       <c r="F8" s="6"/>
       <c r="G8" s="6"/>
       <c r="H8" s="3"/>
@@ -1526,13 +1596,17 @@
         <v>16</v>
       </c>
       <c r="B9" s="10"/>
-      <c r="C9" s="10"/>
+      <c r="C9" s="10" t="s">
+        <v>53</v>
+      </c>
       <c r="D9" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="E9" s="10"/>
+      <c r="E9" s="10" t="s">
+        <v>54</v>
+      </c>
       <c r="F9" s="6"/>
-      <c r="G9" s="7"/>
+      <c r="G9" s="6"/>
       <c r="H9" s="4"/>
       <c r="I9" s="4"/>
       <c r="J9" s="4"/>
@@ -1558,11 +1632,15 @@
         <v>17</v>
       </c>
       <c r="B10" s="10"/>
-      <c r="C10" s="10"/>
+      <c r="C10" s="10" t="s">
+        <v>55</v>
+      </c>
       <c r="D10" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="E10" s="10"/>
+      <c r="E10" s="10" t="s">
+        <v>56</v>
+      </c>
       <c r="F10" s="6"/>
       <c r="G10" s="7"/>
       <c r="H10" s="4"/>
@@ -1590,13 +1668,17 @@
         <v>18</v>
       </c>
       <c r="B11" s="10"/>
-      <c r="C11" s="10"/>
+      <c r="C11" s="10" t="s">
+        <v>45</v>
+      </c>
       <c r="D11" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="E11" s="10"/>
+      <c r="E11" s="10" t="s">
+        <v>46</v>
+      </c>
       <c r="F11" s="6"/>
-      <c r="G11" s="8"/>
+      <c r="G11" s="7"/>
       <c r="H11" s="1"/>
       <c r="I11" s="1"/>
       <c r="J11" s="1"/>
@@ -1622,11 +1704,15 @@
         <v>19</v>
       </c>
       <c r="B12" s="10"/>
-      <c r="C12" s="10"/>
+      <c r="C12" s="10" t="s">
+        <v>51</v>
+      </c>
       <c r="D12" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="E12" s="10"/>
+      <c r="E12" s="10" t="s">
+        <v>52</v>
+      </c>
       <c r="F12" s="6"/>
       <c r="G12" s="8"/>
       <c r="H12" s="1"/>
@@ -1654,11 +1740,15 @@
         <v>20</v>
       </c>
       <c r="B13" s="10"/>
-      <c r="C13" s="10"/>
+      <c r="C13" s="10" t="s">
+        <v>44</v>
+      </c>
       <c r="D13" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="E13" s="10"/>
+      <c r="E13" s="10" t="s">
+        <v>47</v>
+      </c>
       <c r="F13" s="6"/>
       <c r="G13" s="8"/>
       <c r="H13" s="1"/>
@@ -1779,7 +1869,7 @@
     </row>
     <row r="17" spans="1:26" ht="96.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="10" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B17" s="10"/>
       <c r="C17" s="10"/>
@@ -1811,7 +1901,7 @@
     </row>
     <row r="18" spans="1:26" ht="99.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="10" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B18" s="10"/>
       <c r="C18" s="10"/>
@@ -1843,7 +1933,7 @@
     </row>
     <row r="19" spans="1:26" ht="78.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="10" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B19" s="10"/>
       <c r="C19" s="10"/>
@@ -1875,7 +1965,7 @@
     </row>
     <row r="20" spans="1:26" ht="84" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="10" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B20" s="10"/>
       <c r="C20" s="10"/>
@@ -1907,7 +1997,7 @@
     </row>
     <row r="21" spans="1:26" ht="87.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="10" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B21" s="10"/>
       <c r="C21" s="10"/>
@@ -1939,7 +2029,7 @@
     </row>
     <row r="22" spans="1:26" ht="96" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="10" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B22" s="10"/>
       <c r="C22" s="10"/>
@@ -1971,10 +2061,10 @@
     </row>
     <row r="23" spans="1:26" ht="82.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="10" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B23" s="10"/>
-      <c r="C23" s="12"/>
+      <c r="C23" s="10"/>
       <c r="D23" s="10" t="s">
         <v>9</v>
       </c>
@@ -2003,16 +2093,16 @@
     </row>
     <row r="24" spans="1:26" ht="75.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="10" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B24" s="10"/>
       <c r="C24" s="12"/>
       <c r="D24" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="E24" s="12"/>
+      <c r="E24" s="10"/>
       <c r="F24" s="6"/>
-      <c r="G24" s="9"/>
+      <c r="G24" s="8"/>
       <c r="H24" s="1"/>
       <c r="I24" s="1"/>
       <c r="J24" s="1"/>
@@ -2035,7 +2125,7 @@
     </row>
     <row r="25" spans="1:26" ht="84" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="10" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B25" s="10"/>
       <c r="C25" s="12"/>
@@ -2067,10 +2157,10 @@
     </row>
     <row r="26" spans="1:26" ht="94.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="10" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B26" s="10"/>
-      <c r="C26" s="22"/>
+      <c r="C26" s="12"/>
       <c r="D26" s="10" t="s">
         <v>9</v>
       </c>
@@ -2099,10 +2189,10 @@
     </row>
     <row r="27" spans="1:26" ht="103.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="10" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B27" s="10"/>
-      <c r="C27" s="12"/>
+      <c r="C27" s="22"/>
       <c r="D27" s="10" t="s">
         <v>9</v>
       </c>
@@ -2131,14 +2221,14 @@
     </row>
     <row r="28" spans="1:26" ht="96" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" s="10" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B28" s="10"/>
       <c r="C28" s="12"/>
       <c r="D28" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="E28" s="13"/>
+      <c r="E28" s="12"/>
       <c r="F28" s="6"/>
       <c r="G28" s="9"/>
       <c r="H28" s="1"/>
@@ -2162,11 +2252,15 @@
       <c r="Z28" s="1"/>
     </row>
     <row r="29" spans="1:26" ht="97.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="14"/>
+      <c r="A29" s="10" t="s">
+        <v>35</v>
+      </c>
       <c r="B29" s="10"/>
       <c r="C29" s="12"/>
-      <c r="D29" s="10"/>
-      <c r="E29" s="12"/>
+      <c r="D29" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="E29" s="13"/>
       <c r="F29" s="6"/>
       <c r="G29" s="9"/>
       <c r="H29" s="1"/>
@@ -2219,9 +2313,9 @@
     </row>
     <row r="31" spans="1:26" ht="90.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A31" s="14"/>
-      <c r="B31" s="12"/>
+      <c r="B31" s="10"/>
       <c r="C31" s="12"/>
-      <c r="D31" s="12"/>
+      <c r="D31" s="10"/>
       <c r="E31" s="12"/>
       <c r="F31" s="6"/>
       <c r="G31" s="9"/>
@@ -2246,13 +2340,13 @@
       <c r="Z31" s="1"/>
     </row>
     <row r="32" spans="1:26" ht="80.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="11"/>
-      <c r="B32" s="10"/>
-      <c r="C32" s="19"/>
-      <c r="D32" s="17"/>
-      <c r="E32" s="19"/>
-      <c r="F32" s="8"/>
-      <c r="G32" s="8"/>
+      <c r="A32" s="14"/>
+      <c r="B32" s="12"/>
+      <c r="C32" s="12"/>
+      <c r="D32" s="12"/>
+      <c r="E32" s="12"/>
+      <c r="F32" s="6"/>
+      <c r="G32" s="9"/>
       <c r="H32" s="1"/>
       <c r="I32" s="1"/>
       <c r="J32" s="1"/>
@@ -2275,7 +2369,7 @@
     </row>
     <row r="33" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A33" s="11"/>
-      <c r="B33" s="17"/>
+      <c r="B33" s="10"/>
       <c r="C33" s="19"/>
       <c r="D33" s="17"/>
       <c r="E33" s="19"/>
@@ -29070,6 +29164,13 @@
       <c r="Z989" s="1"/>
     </row>
     <row r="990" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A990" s="11"/>
+      <c r="B990" s="17"/>
+      <c r="C990" s="19"/>
+      <c r="D990" s="17"/>
+      <c r="E990" s="19"/>
+      <c r="F990" s="8"/>
+      <c r="G990" s="8"/>
       <c r="H990" s="1"/>
       <c r="I990" s="1"/>
       <c r="J990" s="1"/>
@@ -29095,7 +29196,7 @@
     <mergeCell ref="A1:G2"/>
   </mergeCells>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="F4:F1048575" xr:uid="{00000000-0002-0000-0000-000001000000}">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="F4:F1048576" xr:uid="{00000000-0002-0000-0000-000001000000}">
       <formula1>"Pass,Fail,N/A"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>